<commit_message>
IRB added. 2 or 3 to finish all
</commit_message>
<xml_diff>
--- a/src/Corporate Bond/Export/2022_12_31_Corporate Bonds HO_B 20221231.xlsx
+++ b/src/Corporate Bond/Export/2022_12_31_Corporate Bonds HO_B 20221231.xlsx
@@ -97,21 +97,21 @@
     <t>AT0000A21LB6</t>
   </si>
   <si>
+    <t>XS2181577268</t>
+  </si>
+  <si>
     <t>XS2171872570</t>
   </si>
   <si>
+    <t>AT0000A22H40</t>
+  </si>
+  <si>
     <t>PTGALLOM0004</t>
   </si>
   <si>
-    <t>AT0000A22H40</t>
-  </si>
-  <si>
     <t>AT0000A2GLA0</t>
   </si>
   <si>
-    <t>XS2181577268</t>
-  </si>
-  <si>
     <t>FR0014003G27</t>
   </si>
   <si>
@@ -130,21 +130,21 @@
     <t>695131</t>
   </si>
   <si>
+    <t>152723</t>
+  </si>
+  <si>
     <t>149591</t>
   </si>
   <si>
+    <t>14056</t>
+  </si>
+  <si>
     <t>451118</t>
   </si>
   <si>
-    <t>14056</t>
-  </si>
-  <si>
     <t>1532</t>
   </si>
   <si>
-    <t>152723</t>
-  </si>
-  <si>
     <t>1987280</t>
   </si>
   <si>
@@ -163,21 +163,21 @@
     <t>Breiteneder Immobilien Parking AG</t>
   </si>
   <si>
+    <t>Silgan Holdings Inc.</t>
+  </si>
+  <si>
     <t>Nokia Oyj</t>
   </si>
   <si>
+    <t>CA Immobilien Anlagen;Aktiengesellschaft</t>
+  </si>
+  <si>
     <t>Galp Energia SGPS SA</t>
   </si>
   <si>
-    <t>CA Immobilien Anlagen;Aktiengesellschaft</t>
-  </si>
-  <si>
     <t>Wienerberger AG</t>
   </si>
   <si>
-    <t>Silgan Holdings Inc.</t>
-  </si>
-  <si>
     <t>Verallia SA</t>
   </si>
   <si>
@@ -196,21 +196,21 @@
     <t>720211</t>
   </si>
   <si>
+    <t>221570</t>
+  </si>
+  <si>
     <t>22660</t>
   </si>
   <si>
+    <t>1333543</t>
+  </si>
+  <si>
     <t>715050</t>
   </si>
   <si>
-    <t>1333543</t>
-  </si>
-  <si>
     <t>1293</t>
   </si>
   <si>
-    <t>221570</t>
-  </si>
-  <si>
     <t>868679</t>
   </si>
   <si>
@@ -229,21 +229,21 @@
     <t>Group Breiteneder Immobilien Parking</t>
   </si>
   <si>
+    <t>Group Silgan Holdings</t>
+  </si>
+  <si>
     <t>Group Nokia</t>
   </si>
   <si>
+    <t>Group Starwood Capital</t>
+  </si>
+  <si>
     <t>Group Galp Energia</t>
   </si>
   <si>
-    <t>Group Starwood Capital</t>
-  </si>
-  <si>
     <t>Group Wienerberger</t>
   </si>
   <si>
-    <t>Group Silgan Holdings</t>
-  </si>
-  <si>
     <t>Group Verallia</t>
   </si>
   <si>
@@ -262,15 +262,15 @@
     <t>AT</t>
   </si>
   <si>
+    <t>US</t>
+  </si>
+  <si>
     <t>FI</t>
   </si>
   <si>
     <t>PT</t>
   </si>
   <si>
-    <t>US</t>
-  </si>
-  <si>
     <t>FR</t>
   </si>
   <si>
@@ -286,6 +286,9 @@
     <t>Real Estate &amp; Public Sector - L5*1010251010</t>
   </si>
   <si>
+    <t>Consumer &amp; Life Science - L5*1010401012</t>
+  </si>
+  <si>
     <t>Digital - L5*1010451013</t>
   </si>
   <si>
@@ -295,27 +298,24 @@
     <t>Industrials - L5*1010501010</t>
   </si>
   <si>
-    <t>Consumer &amp; Life Science - L5*1010401012</t>
-  </si>
-  <si>
     <t>WZHKCO</t>
   </si>
   <si>
+    <t>WZHSOBA</t>
+  </si>
+  <si>
     <t>WZHPERI</t>
   </si>
   <si>
+    <t>WZBHUH</t>
+  </si>
+  <si>
     <t>WZHHDE</t>
   </si>
   <si>
-    <t>WZBHUH</t>
-  </si>
-  <si>
     <t>WZBHRH</t>
   </si>
   <si>
-    <t>WZHSOBA</t>
-  </si>
-  <si>
     <t>WZBZMM</t>
   </si>
   <si>
@@ -340,18 +340,18 @@
     <t>CORP_4C</t>
   </si>
   <si>
+    <t>CORPL_4B</t>
+  </si>
+  <si>
     <t>CORPL_3A</t>
   </si>
   <si>
+    <t>CORPL_3C</t>
+  </si>
+  <si>
     <t>CORPL_4A</t>
   </si>
   <si>
-    <t>CORPL_3C</t>
-  </si>
-  <si>
-    <t>CORPL_4B</t>
-  </si>
-  <si>
     <t>CORPL_3B</t>
   </si>
   <si>
@@ -361,15 +361,15 @@
     <t>REAL ESTATE</t>
   </si>
   <si>
+    <t>MATERIALS</t>
+  </si>
+  <si>
     <t>INFORMATION TECHNOLOGY</t>
   </si>
   <si>
     <t>ENERGY</t>
   </si>
   <si>
-    <t>MATERIALS</t>
-  </si>
-  <si>
     <t>INDUSTRIALS</t>
   </si>
   <si>
@@ -379,21 +379,21 @@
     <t>Specialized Real Estate</t>
   </si>
   <si>
+    <t>Metal Containers (formerly Metal &amp; Glas Containers)</t>
+  </si>
+  <si>
     <t>IT Hardware</t>
   </si>
   <si>
+    <t>Real Estate Services</t>
+  </si>
+  <si>
     <t>Integrated Oil &amp; Gas</t>
   </si>
   <si>
-    <t>Real Estate Services</t>
-  </si>
-  <si>
     <t>Construction Materials</t>
   </si>
   <si>
-    <t>Metal Containers (formerly Metal &amp; Glas Containers)</t>
-  </si>
-  <si>
     <t>Glas Containers</t>
   </si>
   <si>
@@ -409,13 +409,13 @@
     <t xml:space="preserve">Activities of head offices  </t>
   </si>
   <si>
+    <t xml:space="preserve">Manufacture of light metal packaging  </t>
+  </si>
+  <si>
     <t xml:space="preserve">Manufacture of consumer electronics  </t>
   </si>
   <si>
     <t xml:space="preserve">Renting and operating of own or leased real estate  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manufacture of light metal packaging  </t>
   </si>
   <si>
     <t xml:space="preserve">Manufacture of hollow glass  </t>
@@ -984,19 +984,19 @@
         <v>82</v>
       </c>
       <c r="H3" s="2">
-        <v>46888</v>
+        <v>46905</v>
       </c>
       <c r="I3">
-        <v>1613527.602213913</v>
+        <v>11689436.35453974</v>
       </c>
       <c r="J3">
-        <v>5495561.82</v>
+        <v>20313607.99203133</v>
       </c>
       <c r="K3">
-        <v>5399810.3</v>
+        <v>20106103.15</v>
       </c>
       <c r="L3">
-        <v>98886.98</v>
+        <v>207500</v>
       </c>
       <c r="M3" t="s">
         <v>87</v>
@@ -1017,7 +1017,7 @@
         <v>108</v>
       </c>
       <c r="S3">
-        <v>0.089</v>
+        <v>0.299</v>
       </c>
       <c r="T3">
         <v>0.45</v>
@@ -1064,19 +1064,19 @@
         <v>83</v>
       </c>
       <c r="H4" s="2">
-        <v>44972</v>
+        <v>46888</v>
       </c>
       <c r="I4">
-        <v>98907.14254398174</v>
+        <v>1613527.602213913</v>
       </c>
       <c r="J4">
-        <v>201890.46</v>
+        <v>5495561.82</v>
       </c>
       <c r="K4">
-        <v>200137.04</v>
+        <v>5399810.3</v>
       </c>
       <c r="L4">
-        <v>1753.42</v>
+        <v>98886.98</v>
       </c>
       <c r="M4" t="s">
         <v>87</v>
@@ -1090,11 +1090,14 @@
       <c r="P4" t="s">
         <v>96</v>
       </c>
+      <c r="Q4" t="s">
+        <v>105</v>
+      </c>
       <c r="R4" t="s">
         <v>109</v>
       </c>
       <c r="S4">
-        <v>0.22</v>
+        <v>0.089</v>
       </c>
       <c r="T4">
         <v>0.45</v>
@@ -1106,7 +1109,7 @@
         <v>122</v>
       </c>
       <c r="W4" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="X4" t="s">
         <v>138</v>
@@ -1183,7 +1186,7 @@
         <v>123</v>
       </c>
       <c r="W5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="X5" t="s">
         <v>138</v>
@@ -1215,22 +1218,22 @@
         <v>74</v>
       </c>
       <c r="G6" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="H6" s="2">
-        <v>45812</v>
+        <v>44972</v>
       </c>
       <c r="I6">
-        <v>443644.0624502721</v>
+        <v>98907.14254398174</v>
       </c>
       <c r="J6">
-        <v>1063779.27</v>
+        <v>201890.46</v>
       </c>
       <c r="K6">
-        <v>1048316.43</v>
+        <v>200137.04</v>
       </c>
       <c r="L6">
-        <v>15897.26</v>
+        <v>1753.42</v>
       </c>
       <c r="M6" t="s">
         <v>87</v>
@@ -1245,10 +1248,10 @@
         <v>98</v>
       </c>
       <c r="R6" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="S6">
-        <v>0.164</v>
+        <v>0.22</v>
       </c>
       <c r="T6">
         <v>0.45</v>
@@ -1292,22 +1295,22 @@
         <v>75</v>
       </c>
       <c r="G7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H7" s="2">
-        <v>46905</v>
+        <v>45812</v>
       </c>
       <c r="I7">
-        <v>11689436.35453974</v>
+        <v>443644.0624502721</v>
       </c>
       <c r="J7">
-        <v>20313607.99203133</v>
+        <v>1063779.27</v>
       </c>
       <c r="K7">
-        <v>20106103.15</v>
+        <v>1048316.43</v>
       </c>
       <c r="L7">
-        <v>207500</v>
+        <v>15897.26</v>
       </c>
       <c r="M7" t="s">
         <v>87</v>
@@ -1321,26 +1324,23 @@
       <c r="P7" t="s">
         <v>99</v>
       </c>
-      <c r="Q7" t="s">
-        <v>105</v>
-      </c>
       <c r="R7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="S7">
-        <v>0.299</v>
+        <v>0.164</v>
       </c>
       <c r="T7">
         <v>0.45</v>
       </c>
       <c r="U7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="V7" t="s">
         <v>125</v>
       </c>
       <c r="W7" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="X7" t="s">
         <v>138</v>
@@ -1396,7 +1396,7 @@
         <v>1</v>
       </c>
       <c r="O8" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="P8" t="s">
         <v>100</v>
@@ -1405,7 +1405,7 @@
         <v>105</v>
       </c>
       <c r="R8" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="S8">
         <v>0.22</v>
@@ -1414,7 +1414,7 @@
         <v>0.45</v>
       </c>
       <c r="U8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="V8" t="s">
         <v>126</v>
@@ -1476,7 +1476,7 @@
         <v>1</v>
       </c>
       <c r="O9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="P9" t="s">
         <v>101</v>
@@ -1532,7 +1532,7 @@
         <v>78</v>
       </c>
       <c r="G10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H10" s="2">
         <v>45366</v>
@@ -1556,7 +1556,7 @@
         <v>1</v>
       </c>
       <c r="O10" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="P10" t="s">
         <v>102</v>
@@ -1565,7 +1565,7 @@
         <v>105</v>
       </c>
       <c r="R10" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="S10">
         <v>0.22</v>
@@ -1574,10 +1574,10 @@
         <v>0.45</v>
       </c>
       <c r="U10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="V10" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="W10" t="s">
         <v>136</v>
@@ -1636,7 +1636,7 @@
         <v>1.1274846944</v>
       </c>
       <c r="O11" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="P11" t="s">
         <v>103</v>
@@ -1737,7 +1737,7 @@
         <v>129</v>
       </c>
       <c r="W12" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="X12" t="s">
         <v>138</v>

</xml_diff>